<commit_message>
Fixed LoadProhibited error in wire. Must use header only for programflow.h
</commit_message>
<xml_diff>
--- a/Codebase/TestLog.xlsx
+++ b/Codebase/TestLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Caving\BenBoi\SurveyingDevice\Codebase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83DE9E8-AFC5-4CBF-8C35-0433D22C5FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C180FD61-3197-4D6E-9922-44F5A68F0285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{638C6D99-3177-4D78-9889-01E0112FD6A6}"/>
+    <workbookView xWindow="708" yWindow="708" windowWidth="20148" windowHeight="12012" xr2:uid="{638C6D99-3177-4D78-9889-01E0112FD6A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Type</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>displaySaveCalibYN</t>
+  </si>
+  <si>
+    <t>displayNewCalibYN</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7917DC0-AA4C-43E1-A9EB-678AD58D2506}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,6 +565,24 @@
       </c>
       <c r="D8" s="1"/>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>